<commit_message>
Added AutomationInstances for Omega on MD
</commit_message>
<xml_diff>
--- a/Cmf.Custom.Tests/MasterData/Files/30000-MasterData-IoT.xlsx
+++ b/Cmf.Custom.Tests/MasterData/Files/30000-MasterData-IoT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CMF\projects\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gits\AMSOSRAM\Cmf.Custom.Tests\MasterData\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF74DE28-40A7-4199-BE70-B9A64BCBA2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140B6BC8-0692-482D-9793-F5F3DA45CC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8295" yWindow="2175" windowWidth="21600" windowHeight="11235" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="465">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="467">
   <si>
     <t>Tab Name</t>
   </si>
@@ -1497,6 +1497,12 @@
   </si>
   <si>
     <t>5FICP1</t>
+  </si>
+  <si>
+    <t>5FICP1.RFID</t>
+  </si>
+  <si>
+    <t>OmegaPlasmaController</t>
   </si>
 </sst>
 </file>
@@ -1531,10 +1537,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3616,8 +3623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3775,11 +3782,19 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3947,6 +3962,49 @@
       <c r="D13" s="1" t="s">
         <v>450</v>
       </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="D17" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>